<commit_message>
commit with 9 testcases
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData_QALegend.xlsx
+++ b/src/main/resources/TestData_QALegend.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\com.qalegendbilling\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A58271-8724-4420-8D62-EAFB591335B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E573C4-D011-4A83-BE64-CABB0A3D5D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="1260" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5124" yWindow="3708" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="UserManagemntOptions" sheetId="3" r:id="rId2"/>
     <sheet name="UserPage" sheetId="4" r:id="rId3"/>
-    <sheet name="ResetPage" sheetId="2" r:id="rId4"/>
+    <sheet name="ViewUserPage" sheetId="5" r:id="rId4"/>
+    <sheet name="ResetPage" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>aryav</t>
   </si>
@@ -76,6 +77,24 @@
   </si>
   <si>
     <t>No matching records found</t>
+  </si>
+  <si>
+    <t>Email:</t>
+  </si>
+  <si>
+    <t>Role:</t>
+  </si>
+  <si>
+    <t>Username:</t>
+  </si>
+  <si>
+    <t>Sales Commission Percentage (%):</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Allowed Contacts: All</t>
   </si>
 </sst>
 </file>
@@ -500,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379458C8-229F-4A93-825B-B9C99D63EC2D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -525,6 +544,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D33AF0-C860-47FA-A05F-93D241652263}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C690E3-D4BC-4ED7-B885-A8C108594FEB}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>